<commit_message>
fix delete sales order
</commit_message>
<xml_diff>
--- a/sample/sample_sales_order.xlsx
+++ b/sample/sample_sales_order.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documents\Kantor\Sample Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39BEBC15-7869-434A-8A1A-79D5560CB3D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383DD66B-B064-401C-A7EE-8D76A769A320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upload sales order" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
-  <si>
-    <t>NO. PAJAK</t>
-  </si>
-  <si>
-    <t>kode toko</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>NAMA PELANGGAN</t>
   </si>
@@ -92,12 +86,27 @@
   </si>
   <si>
     <t>LT 7.50-16 14PR SU 88N</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>NO. FAKTUR</t>
+  </si>
+  <si>
+    <t>KODE TOKO</t>
+  </si>
+  <si>
+    <t>1. JIKA NO FAKTUR 24.0000024 MAKA HARUS DITAMBAHKAN SERI PAJAK DIDEPANNYA, SUPAYA SERI NO FAKTUR SAMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAGIAN INI HAPUS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +421,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -575,8 +590,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -931,11 +947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,140 +966,155 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>